<commit_message>
a pics and ref
</commit_message>
<xml_diff>
--- a/doc/财务记录/XDM-I研发采购18年7-9月.xlsx
+++ b/doc/财务记录/XDM-I研发采购18年7-9月.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>备注</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -96,6 +96,17 @@
   </si>
   <si>
     <t>多种</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树莓派1套</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://item.taobao.com/item.htm?spm=a1z09.2.0.0.2b962e8dlwdNUv&amp;id=527576110046&amp;_u=e3s1sni8961</t>
+  </si>
+  <si>
+    <t>联东U谷停车费</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -455,11 +466,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H32" sqref="H32"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -611,23 +622,52 @@
       </c>
     </row>
     <row r="7" spans="2:9">
-      <c r="C7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="B7">
+        <v>20180820</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>280</v>
+      </c>
     </row>
     <row r="8" spans="2:9">
+      <c r="B8">
+        <v>20180913</v>
+      </c>
       <c r="C8" s="1"/>
+      <c r="D8" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="E8" s="1"/>
+      <c r="H8">
+        <v>17.5</v>
+      </c>
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="2:9">
       <c r="C9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="2:9">
       <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="2:9">
       <c r="C11" s="1"/>
@@ -640,24 +680,22 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
     </row>
     <row r="13" spans="2:9">
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="2:9">
       <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
     </row>
     <row r="15" spans="2:9">
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
     </row>
     <row r="16" spans="2:9">
       <c r="C16" s="1"/>
@@ -668,13 +706,15 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
     </row>
     <row r="18" spans="3:9">
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="3:9">
       <c r="C19" s="1"/>
@@ -701,15 +741,13 @@
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
     </row>
     <row r="23" spans="3:9">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
     </row>
     <row r="24" spans="3:9">
       <c r="C24" s="1"/>
@@ -730,57 +768,60 @@
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
+      <c r="I27" s="1"/>
     </row>
     <row r="28" spans="3:9">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="I28" s="1"/>
     </row>
     <row r="29" spans="3:9">
       <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
     <row r="30" spans="3:9">
       <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
     <row r="31" spans="3:9">
       <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
     <row r="32" spans="3:9">
       <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
     <row r="33" spans="1:9">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:9">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
     </row>
     <row r="35" spans="1:9">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
     </row>
     <row r="36" spans="1:9">
       <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
+      <c r="I36" s="1"/>
     </row>
     <row r="37" spans="1:9">
       <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -792,27 +833,19 @@
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
-      <c r="I38" s="1"/>
     </row>
     <row r="39" spans="1:9">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="42" spans="1:9">
-      <c r="A42" s="1" t="s">
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H42">
-        <f>SUM(H2:H41)</f>
-        <v>225.67000000000002</v>
+      <c r="H41">
+        <f>SUM(H2:H40)</f>
+        <v>523.17000000000007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>